<commit_message>
[Mod][Client] - UPDATE dailyscrum2
</commit_message>
<xml_diff>
--- a/Client/[AudioPipe][26-11-12]DailyScrum2.xlsx
+++ b/Client/[AudioPipe][26-11-12]DailyScrum2.xlsx
@@ -359,8 +359,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18586844050258686"/>
-          <c:y val="1.7259978425026967E-2"/>
+          <c:x val="0.18586844050258691"/>
+          <c:y val="1.7259978425026964E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -373,7 +373,7 @@
           <c:x val="4.9222842871136832E-2"/>
           <c:y val="0.12821649720969344"/>
           <c:w val="0.81920541983534112"/>
-          <c:h val="0.77895166016869299"/>
+          <c:h val="0.77895166016869322"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -431,6 +431,15 @@
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,23 +532,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="74040832"/>
-        <c:axId val="74042368"/>
+        <c:axId val="79869440"/>
+        <c:axId val="79870976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74040832"/>
+        <c:axId val="79869440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74042368"/>
+        <c:crossAx val="79870976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74042368"/>
+        <c:axId val="79870976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +556,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74040832"/>
+        <c:crossAx val="79869440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -560,7 +569,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -888,7 +897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1021,7 +1032,9 @@
       <c r="E3" s="16">
         <v>1</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -1061,9 +1074,15 @@
       <c r="E4" s="17">
         <v>2</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="F4" s="17">
+        <v>2</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>2</v>
+      </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
@@ -1103,9 +1122,15 @@
       <c r="E5" s="16">
         <v>1</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="F5" s="16">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16">
+        <v>1</v>
+      </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
@@ -1147,9 +1172,15 @@
       <c r="E6" s="17">
         <v>1</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
@@ -1190,15 +1221,15 @@
       </c>
       <c r="F7" s="10">
         <f>SUM(F3:F6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" ref="G7:M7" si="0">SUM(G3:G6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="0"/>
@@ -1429,9 +1460,15 @@
       <c r="E11" s="17">
         <v>2</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="F11" s="17">
+        <v>2</v>
+      </c>
+      <c r="G11" s="17">
+        <v>2</v>
+      </c>
+      <c r="H11" s="17">
+        <v>2</v>
+      </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -1477,9 +1514,15 @@
       <c r="E12" s="17">
         <v>2</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="F12" s="17">
+        <v>2</v>
+      </c>
+      <c r="G12" s="17">
+        <v>2</v>
+      </c>
+      <c r="H12" s="17">
+        <v>2</v>
+      </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -1529,9 +1572,15 @@
       <c r="E13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="F13" s="17">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2</v>
+      </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -1583,9 +1632,15 @@
       <c r="E14" s="16">
         <v>1</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
@@ -1629,85 +1684,85 @@
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3">
-        <f>SUM(E10:E14)</f>
+        <f t="shared" ref="E15:N15" si="3">SUM(E10:E14)</f>
         <v>8</v>
       </c>
       <c r="F15" s="3">
-        <f>SUM(F10:F14)</f>
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G15" s="3">
-        <f>SUM(G10:G14)</f>
+      <c r="J15" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H15" s="3">
-        <f>SUM(H10:H14)</f>
+      <c r="K15" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I15" s="3">
-        <f>SUM(I10:I14)</f>
+      <c r="L15" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J15" s="3">
-        <f>SUM(J10:J14)</f>
+      <c r="M15" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K15" s="3">
-        <f>SUM(K10:K14)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
-        <f>SUM(L10:L14)</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="3">
-        <f>SUM(M10:M14)</f>
-        <v>0</v>
-      </c>
       <c r="N15" s="3">
-        <f>SUM(N10:N14)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="3">
-        <f>SUM(Q10:Q14)</f>
+        <f t="shared" ref="Q15:Z15" si="4">SUM(Q10:Q14)</f>
         <v>8</v>
       </c>
       <c r="R15" s="3">
-        <f>SUM(R10:R14)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="S15" s="3">
-        <f>SUM(S10:S14)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="T15" s="3">
-        <f>SUM(T10:T14)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="U15" s="3">
-        <f>SUM(U10:U14)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="V15" s="3">
-        <f>SUM(V10:V14)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="W15" s="3">
-        <f>SUM(W10:W14)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="X15" s="3">
-        <f>SUM(X10:X14)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="Y15" s="3">
-        <f>SUM(Y10:Y14)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Z15" s="3">
-        <f>SUM(Z10:Z14)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1885,8 +1940,12 @@
       <c r="E20" s="16">
         <v>1</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -1933,8 +1992,12 @@
       <c r="E21" s="17">
         <v>1</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="F21" s="17">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17">
+        <v>1</v>
+      </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -1984,38 +2047,38 @@
       </c>
       <c r="F22" s="10">
         <f>SUM(F20:F21)</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" ref="G22:N22" si="5">SUM(G20:G21)</f>
+        <v>2</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G22" s="10">
-        <f t="shared" ref="G22:N22" si="3">SUM(G20:G21)</f>
+      <c r="I22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H22" s="10">
-        <f t="shared" si="3"/>
+      <c r="J22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I22" s="10">
-        <f t="shared" si="3"/>
+      <c r="K22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J22" s="10">
-        <f t="shared" si="3"/>
+      <c r="L22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K22" s="10">
-        <f t="shared" si="3"/>
+      <c r="M22" s="10">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L22" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="N22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O22" s="1"/>
@@ -2029,35 +2092,35 @@
         <v>2</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" ref="S22:Z22" si="4">SUM(S20:S21)</f>
+        <f t="shared" ref="S22:Z22" si="6">SUM(S20:S21)</f>
         <v>2</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="V22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="W22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="X22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Y22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Z22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2072,48 +2135,60 @@
         <f>E22+E15+E7</f>
         <v>15</v>
       </c>
+      <c r="F23">
+        <f t="shared" ref="F23:H23" si="7">F22+F15+F7</f>
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="Q23">
-        <f>Q22+Q15+Q7</f>
+        <f t="shared" ref="Q23:Z23" si="8">Q22+Q15+Q7</f>
         <v>15</v>
       </c>
       <c r="R23">
-        <f>R22+R15+R7</f>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="S23">
-        <f>S22+S15+S7</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="T23">
-        <f>T22+T15+T7</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="U23">
-        <f>U22+U15+U7</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="V23">
-        <f>V22+V15+V7</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="W23">
-        <f>W22+W15+W7</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="X23">
-        <f>X22+X15+X7</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="Y23">
-        <f>Y22+Y15+Y7</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="Z23">
-        <f>Z22+Z15+Z7</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -2208,7 +2283,7 @@
     <row r="27" spans="1:26">
       <c r="A27" s="1"/>
       <c r="B27" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -2482,7 +2557,7 @@
       </c>
       <c r="C36" s="1" t="str">
         <f>IF(B27&gt;=B33,"OK - Temps de travail","ERREUR - Temps de travail")</f>
-        <v>OK - Temps de travail</v>
+        <v>ERREUR - Temps de travail</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>

</xml_diff>